<commit_message>
Update Tractor Sales Excel Forecasting.xlsx
</commit_message>
<xml_diff>
--- a/Tractor Sales Excel Forecasting.xlsx
+++ b/Tractor Sales Excel Forecasting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Week1_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21E329EB-AB4E-45B1-A7AE-5BB3D52E7D39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E29FFB4-ACE0-4138-8AC6-86B46C2F2D77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="71895" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{10D37E4D-5CAB-4CAE-9598-6961AD2CA259}"/>
   </bookViews>
@@ -5191,7 +5191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0FE46F-7D9B-42C4-9E97-703E9A32EDED}">
   <dimension ref="A1:L191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -19034,16 +19034,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51E67886-47CC-48E2-BDDD-8A804DC20AB3}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="eb7c3fc1-ccd5-477b-94a4-7b6dc96a8d59"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="eb7c3fc1-ccd5-477b-94a4-7b6dc96a8d59"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="9e706368-9a73-4dcc-9221-b8fc62424fbc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9e706368-9a73-4dcc-9221-b8fc62424fbc"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>